<commit_message>
some date format changes
</commit_message>
<xml_diff>
--- a/employee_details.xlsx
+++ b/employee_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patol\OneDrive\Desktop\Movya\BdayFestivalWishes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55627948-38F5-41A6-BBA8-3E1DA9930F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA09F450-5317-4268-82B8-88C7A56AF3CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1213,19 +1213,22 @@
     <t>ppoppy2r@purevolume.com</t>
   </si>
   <si>
-    <t>2004-08-03</t>
-  </si>
-  <si>
     <t>2020-04-17</t>
   </si>
   <si>
     <t>2002-08-16</t>
+  </si>
+  <si>
+    <t>2024-08-20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-14009]yyyy/mm/dd;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1253,8 +1256,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1571,8 +1575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="F91" sqref="F91"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1580,7 +1584,7 @@
     <col min="1" max="1" width="6.4140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.4140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.9140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.9140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.9140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1593,10 +1597,10 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1610,10 +1614,10 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1627,10 +1631,10 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1644,10 +1648,10 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1661,10 +1665,10 @@
       <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1678,10 +1682,10 @@
       <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1695,10 +1699,10 @@
       <c r="C7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1712,10 +1716,10 @@
       <c r="C8" t="s">
         <v>30</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1729,10 +1733,10 @@
       <c r="C9" t="s">
         <v>34</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1746,10 +1750,10 @@
       <c r="C10" t="s">
         <v>38</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1763,10 +1767,10 @@
       <c r="C11" t="s">
         <v>42</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1780,10 +1784,10 @@
       <c r="C12" t="s">
         <v>46</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1797,10 +1801,10 @@
       <c r="C13" t="s">
         <v>50</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1814,10 +1818,10 @@
       <c r="C14" t="s">
         <v>54</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1831,10 +1835,10 @@
       <c r="C15" t="s">
         <v>58</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1848,10 +1852,10 @@
       <c r="C16" t="s">
         <v>62</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1865,10 +1869,10 @@
       <c r="C17" t="s">
         <v>66</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1882,10 +1886,10 @@
       <c r="C18" t="s">
         <v>70</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="1" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1899,10 +1903,10 @@
       <c r="C19" t="s">
         <v>74</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1916,10 +1920,10 @@
       <c r="C20" t="s">
         <v>78</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="1" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1933,10 +1937,10 @@
       <c r="C21" t="s">
         <v>82</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="1" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1950,10 +1954,10 @@
       <c r="C22" t="s">
         <v>86</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="1" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1967,10 +1971,10 @@
       <c r="C23" t="s">
         <v>90</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="1" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1984,10 +1988,10 @@
       <c r="C24" t="s">
         <v>94</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="1" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2001,10 +2005,10 @@
       <c r="C25" t="s">
         <v>98</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="1" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2018,10 +2022,10 @@
       <c r="C26" t="s">
         <v>102</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="1" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2035,10 +2039,10 @@
       <c r="C27" t="s">
         <v>106</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="1" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2052,10 +2056,10 @@
       <c r="C28" t="s">
         <v>110</v>
       </c>
-      <c r="D28" t="s">
-        <v>399</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="D28" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2069,10 +2073,10 @@
       <c r="C29" t="s">
         <v>113</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="1" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2086,10 +2090,10 @@
       <c r="C30" t="s">
         <v>117</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="1" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2103,10 +2107,10 @@
       <c r="C31" t="s">
         <v>121</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="1" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2120,10 +2124,10 @@
       <c r="C32" t="s">
         <v>125</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="1" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2137,10 +2141,10 @@
       <c r="C33" t="s">
         <v>129</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="1" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2154,10 +2158,10 @@
       <c r="C34" t="s">
         <v>133</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="1" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2171,10 +2175,10 @@
       <c r="C35" t="s">
         <v>137</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="1" t="s">
         <v>139</v>
       </c>
     </row>
@@ -2188,10 +2192,10 @@
       <c r="C36" t="s">
         <v>141</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="1" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2205,10 +2209,10 @@
       <c r="C37" t="s">
         <v>145</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="1" t="s">
         <v>147</v>
       </c>
     </row>
@@ -2222,10 +2226,10 @@
       <c r="C38" t="s">
         <v>149</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="1" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2239,10 +2243,10 @@
       <c r="C39" t="s">
         <v>153</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="1" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2256,10 +2260,10 @@
       <c r="C40" t="s">
         <v>157</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="1" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2273,10 +2277,10 @@
       <c r="C41" t="s">
         <v>161</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="1" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2290,10 +2294,10 @@
       <c r="C42" t="s">
         <v>165</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="1" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2307,10 +2311,10 @@
       <c r="C43" t="s">
         <v>169</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="1" t="s">
         <v>171</v>
       </c>
     </row>
@@ -2324,10 +2328,10 @@
       <c r="C44" t="s">
         <v>173</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="1" t="s">
         <v>175</v>
       </c>
     </row>
@@ -2341,10 +2345,10 @@
       <c r="C45" t="s">
         <v>177</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="1" t="s">
         <v>179</v>
       </c>
     </row>
@@ -2358,10 +2362,10 @@
       <c r="C46" t="s">
         <v>181</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="1" t="s">
         <v>183</v>
       </c>
     </row>
@@ -2375,10 +2379,10 @@
       <c r="C47" t="s">
         <v>185</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="1" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2392,10 +2396,10 @@
       <c r="C48" t="s">
         <v>189</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="1" t="s">
         <v>191</v>
       </c>
     </row>
@@ -2409,10 +2413,10 @@
       <c r="C49" t="s">
         <v>193</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="1" t="s">
         <v>195</v>
       </c>
     </row>
@@ -2426,10 +2430,10 @@
       <c r="C50" t="s">
         <v>197</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="1" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2443,10 +2447,10 @@
       <c r="C51" t="s">
         <v>201</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="1" t="s">
         <v>203</v>
       </c>
     </row>
@@ -2460,10 +2464,10 @@
       <c r="C52" t="s">
         <v>205</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="1" t="s">
         <v>207</v>
       </c>
     </row>
@@ -2477,10 +2481,10 @@
       <c r="C53" t="s">
         <v>209</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="1" t="s">
         <v>211</v>
       </c>
     </row>
@@ -2494,10 +2498,10 @@
       <c r="C54" t="s">
         <v>213</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="1" t="s">
         <v>215</v>
       </c>
     </row>
@@ -2511,10 +2515,10 @@
       <c r="C55" t="s">
         <v>217</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="1" t="s">
         <v>219</v>
       </c>
     </row>
@@ -2528,10 +2532,10 @@
       <c r="C56" t="s">
         <v>221</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="1" t="s">
         <v>223</v>
       </c>
     </row>
@@ -2545,10 +2549,10 @@
       <c r="C57" t="s">
         <v>225</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="1" t="s">
         <v>227</v>
       </c>
     </row>
@@ -2562,10 +2566,10 @@
       <c r="C58" t="s">
         <v>229</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="1" t="s">
         <v>231</v>
       </c>
     </row>
@@ -2579,10 +2583,10 @@
       <c r="C59" t="s">
         <v>233</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59" s="1" t="s">
         <v>235</v>
       </c>
     </row>
@@ -2596,10 +2600,10 @@
       <c r="C60" t="s">
         <v>237</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="1" t="s">
         <v>239</v>
       </c>
     </row>
@@ -2613,10 +2617,10 @@
       <c r="C61" t="s">
         <v>241</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="1" t="s">
         <v>243</v>
       </c>
     </row>
@@ -2630,10 +2634,10 @@
       <c r="C62" t="s">
         <v>245</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E62" s="1" t="s">
         <v>247</v>
       </c>
     </row>
@@ -2647,10 +2651,10 @@
       <c r="C63" t="s">
         <v>249</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="1" t="s">
         <v>251</v>
       </c>
     </row>
@@ -2664,10 +2668,10 @@
       <c r="C64" t="s">
         <v>253</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="1" t="s">
         <v>255</v>
       </c>
     </row>
@@ -2681,10 +2685,10 @@
       <c r="C65" t="s">
         <v>257</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E65" s="1" t="s">
         <v>259</v>
       </c>
     </row>
@@ -2698,10 +2702,10 @@
       <c r="C66" t="s">
         <v>261</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66" s="1" t="s">
         <v>263</v>
       </c>
     </row>
@@ -2715,10 +2719,10 @@
       <c r="C67" t="s">
         <v>265</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67" s="1" t="s">
         <v>267</v>
       </c>
     </row>
@@ -2732,10 +2736,10 @@
       <c r="C68" t="s">
         <v>269</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68" s="1" t="s">
         <v>271</v>
       </c>
     </row>
@@ -2749,10 +2753,10 @@
       <c r="C69" t="s">
         <v>273</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69" s="1" t="s">
         <v>275</v>
       </c>
     </row>
@@ -2766,10 +2770,10 @@
       <c r="C70" t="s">
         <v>277</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70" s="1" t="s">
         <v>279</v>
       </c>
     </row>
@@ -2783,10 +2787,10 @@
       <c r="C71" t="s">
         <v>281</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E71" s="1" t="s">
         <v>283</v>
       </c>
     </row>
@@ -2800,10 +2804,10 @@
       <c r="C72" t="s">
         <v>285</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72" s="1" t="s">
         <v>287</v>
       </c>
     </row>
@@ -2817,10 +2821,10 @@
       <c r="C73" t="s">
         <v>289</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E73" s="1" t="s">
         <v>291</v>
       </c>
     </row>
@@ -2834,10 +2838,10 @@
       <c r="C74" t="s">
         <v>293</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74" s="1" t="s">
         <v>295</v>
       </c>
     </row>
@@ -2851,10 +2855,10 @@
       <c r="C75" t="s">
         <v>297</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E75" s="1" t="s">
         <v>299</v>
       </c>
     </row>
@@ -2868,10 +2872,10 @@
       <c r="C76" t="s">
         <v>301</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="1" t="s">
         <v>303</v>
       </c>
     </row>
@@ -2885,10 +2889,10 @@
       <c r="C77" t="s">
         <v>305</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="1" t="s">
         <v>307</v>
       </c>
     </row>
@@ -2902,10 +2906,10 @@
       <c r="C78" t="s">
         <v>309</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E78" s="1" t="s">
         <v>311</v>
       </c>
     </row>
@@ -2919,10 +2923,10 @@
       <c r="C79" t="s">
         <v>313</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D79" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" s="1" t="s">
         <v>314</v>
       </c>
     </row>
@@ -2936,10 +2940,10 @@
       <c r="C80" t="s">
         <v>316</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D80" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E80" s="1" t="s">
         <v>318</v>
       </c>
     </row>
@@ -2953,10 +2957,10 @@
       <c r="C81" t="s">
         <v>320</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D81" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E81" s="1" t="s">
         <v>321</v>
       </c>
     </row>
@@ -2970,10 +2974,10 @@
       <c r="C82" t="s">
         <v>323</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D82" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E82" s="1" t="s">
         <v>325</v>
       </c>
     </row>
@@ -2987,10 +2991,10 @@
       <c r="C83" t="s">
         <v>327</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D83" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E83" s="1" t="s">
         <v>329</v>
       </c>
     </row>
@@ -3004,10 +3008,10 @@
       <c r="C84" t="s">
         <v>331</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D84" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E84" s="1" t="s">
         <v>333</v>
       </c>
     </row>
@@ -3021,10 +3025,10 @@
       <c r="C85" t="s">
         <v>335</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D85" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E85" s="1" t="s">
         <v>337</v>
       </c>
     </row>
@@ -3038,10 +3042,10 @@
       <c r="C86" t="s">
         <v>339</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D86" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E86" s="1" t="s">
         <v>341</v>
       </c>
     </row>
@@ -3055,10 +3059,10 @@
       <c r="C87" t="s">
         <v>343</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E87" s="1" t="s">
         <v>345</v>
       </c>
     </row>
@@ -3072,10 +3076,10 @@
       <c r="C88" t="s">
         <v>347</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D88" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E88" s="1" t="s">
         <v>349</v>
       </c>
     </row>
@@ -3089,10 +3093,10 @@
       <c r="C89" t="s">
         <v>351</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D89" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="E89" t="s">
+      <c r="E89" s="1" t="s">
         <v>353</v>
       </c>
     </row>
@@ -3106,10 +3110,10 @@
       <c r="C90" t="s">
         <v>355</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D90" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E90" s="1" t="s">
         <v>357</v>
       </c>
     </row>
@@ -3123,10 +3127,10 @@
       <c r="C91" t="s">
         <v>359</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D91" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="E91" t="s">
+      <c r="E91" s="1" t="s">
         <v>361</v>
       </c>
     </row>
@@ -3140,10 +3144,10 @@
       <c r="C92" t="s">
         <v>363</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E92" s="1" t="s">
         <v>365</v>
       </c>
     </row>
@@ -3157,10 +3161,10 @@
       <c r="C93" t="s">
         <v>367</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="E93" t="s">
+      <c r="E93" s="1" t="s">
         <v>394</v>
       </c>
     </row>
@@ -3174,10 +3178,10 @@
       <c r="C94" t="s">
         <v>370</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E94" s="1" t="s">
         <v>372</v>
       </c>
     </row>
@@ -3191,10 +3195,10 @@
       <c r="C95" t="s">
         <v>374</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D95" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="E95" t="s">
+      <c r="E95" s="1" t="s">
         <v>376</v>
       </c>
     </row>
@@ -3208,10 +3212,10 @@
       <c r="C96" t="s">
         <v>378</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E96" s="1" t="s">
         <v>380</v>
       </c>
     </row>
@@ -3225,10 +3229,10 @@
       <c r="C97" t="s">
         <v>382</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E97" s="1" t="s">
         <v>384</v>
       </c>
     </row>
@@ -3242,10 +3246,10 @@
       <c r="C98" t="s">
         <v>386</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E98" s="1" t="s">
         <v>394</v>
       </c>
     </row>
@@ -3259,10 +3263,10 @@
       <c r="C99" t="s">
         <v>389</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E99" s="1" t="s">
         <v>391</v>
       </c>
     </row>
@@ -3276,10 +3280,10 @@
       <c r="C100" t="s">
         <v>393</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="E100" t="s">
+      <c r="E100" s="1" t="s">
         <v>372</v>
       </c>
     </row>
@@ -3293,11 +3297,11 @@
       <c r="C101" t="s">
         <v>396</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D101" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="E101" s="1" t="s">
         <v>397</v>
-      </c>
-      <c r="E101" t="s">
-        <v>398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>